<commit_message>
**Title:** Load route numbers from consolidation folder and generate schedule files
- Updated `driver_scheduler.py` to read route numbers from `/consolidation/route_numbers.txt`
- Added logic in `driver_scheduler.py` to generate output files `Расписание_Итог_*` for each route and day
- Modified `config.py` to include path configuration for `route_numbers.txt` file
- Enhanced file generation workflow to dynamically create Excel outputs based on loaded route numbers
- Improved error handling and logging during file creation process

The system now correctly loads route numbers from the consolidation directory and generates individual schedule files for each route and day, ensuring up-to-date and accurate output.
</commit_message>
<xml_diff>
--- a/output/20/Расписание_Итог_1.xlsx
+++ b/output/20/Расписание_Итог_1.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="23040" windowHeight="10500" tabRatio="924" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Расписание" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Расписание" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1" refMode="R1C1"/>

</xml_diff>